<commit_message>
table: add support for column formula
</commit_message>
<xml_diff>
--- a/tests/input/table10.xlsx
+++ b/tests/input/table10.xlsx
@@ -106,7 +106,9 @@
     <tableColumn id="7" name="Column7" totalsRowFunction="min"/>
     <tableColumn id="8" name="Column8" totalsRowFunction="sum"/>
     <tableColumn id="9" name="Column9" totalsRowFunction="stdDev"/>
-    <tableColumn id="10" name="Column10" totalsRowFunction="var"/>
+    <tableColumn id="10" name="Column10" totalsRowFunction="var">
+      <calculatedColumnFormula>SUM(Table1[[#This Row],[Column1]:[Column3]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>